<commit_message>
YNY_REPORTS:KN: 2 new columns (ESP + catchups). Fixe date & time format
</commit_message>
<xml_diff>
--- a/apps/templates/xlsx/kn.xlsx
+++ b/apps/templates/xlsx/kn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>First Name</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Trainer Sessions taken</t>
+  </si>
+  <si>
+    <t>Catchups taken</t>
+  </si>
+  <si>
+    <t>ESP</t>
   </si>
   <si>
     <t>Study total hours</t>
@@ -210,7 +216,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -244,38 +250,38 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="AF11" activeCellId="0" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.5102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.2244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.0612244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="31" min="29" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="31" min="29" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -374,6 +380,12 @@
       </c>
       <c r="AF1" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="ALY1" s="4"/>
       <c r="ALZ1" s="4"/>

</xml_diff>